<commit_message>
HW3 done minus writeup!
</commit_message>
<xml_diff>
--- a/HW3/Outputs/IterationTable.xlsx
+++ b/HW3/Outputs/IterationTable.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\child\Documents\Projects\Optimization\HW3\Outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchild25\Documents\Projects\Optimization\HW3\Outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39068371-56CA-4FA9-A685-DEF3AC9A0644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE855607-C068-47BD-BB46-056E34455BB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{06A4CB9D-E381-4F0B-B1C5-53A6C7289F04}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="12225" xr2:uid="{06A4CB9D-E381-4F0B-B1C5-53A6C7289F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -53,8 +52,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -82,8 +89,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,9 +110,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -142,7 +150,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -248,7 +256,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -390,7 +398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -401,34 +409,34 @@
   <dimension ref="A2:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
@@ -438,41 +446,41 @@
         <v>231</v>
       </c>
       <c r="D3">
-        <v>162</v>
+        <v>79</v>
       </c>
       <c r="E3">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>87250</v>
+        <v>16057</v>
       </c>
       <c r="C4">
-        <v>125764</v>
+        <v>6302</v>
       </c>
       <c r="D4">
-        <v>45356</v>
+        <v>235</v>
       </c>
       <c r="E4">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>3644</v>
+        <v>318</v>
       </c>
       <c r="C5">
-        <v>66262</v>
+        <v>201</v>
       </c>
       <c r="D5">
-        <v>16248</v>
+        <v>134</v>
       </c>
       <c r="E5">
         <v>43</v>
@@ -516,5 +524,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>